<commit_message>
cambios en task contraorden cheque
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,12 @@
     <t>numeroCheque</t>
   </si>
   <si>
+    <t>rangoDesde</t>
+  </si>
+  <si>
+    <t>rangoHasta</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -73,7 +79,7 @@
     <t>Cédula de ciudadanía</t>
   </si>
   <si>
-    <t>testing10</t>
+    <t>zcreditos10</t>
   </si>
   <si>
     <t>1234</t>
@@ -103,7 +109,7 @@
     <t>Corriente</t>
   </si>
   <si>
-    <t>406-139740-01</t>
+    <t>406-158690-06</t>
   </si>
   <si>
     <t>Cheque</t>
@@ -117,9 +123,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -146,6 +152,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -153,7 +166,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,39 +196,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,22 +259,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,31 +275,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,85 +316,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,97 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,28 +537,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,6 +558,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -583,15 +578,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -625,163 +611,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
@@ -1132,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -1152,7 +1162,7 @@
     <col min="15" max="15" width="27.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1183,10 +1193,10 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
@@ -1201,113 +1211,127 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="38" customHeight="1" spans="1:16">
-      <c r="A2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>17</v>
+    <row r="2" s="1" customFormat="1" ht="38" customHeight="1" spans="1:18">
+      <c r="A2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3210</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="38" customHeight="1" spans="1:18">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="F3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="J3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="K3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="L3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="38" customHeight="1" spans="1:16">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N3" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P3" s="1">
         <v>2</v>
       </c>
+      <c r="Q3" s="4">
+        <v>3211</v>
+      </c>
+      <c r="R3" s="4">
+        <v>3216</v>
+      </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="15.75" spans="2:7">
-      <c r="B4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
cambio mapeo para ios actualizar datos de seguridad
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/cheque/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FA3C43-27F2-4A79-B63E-E6345D096C23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -124,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,28 +531,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="10" width="23.453125" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625"/>
-    <col min="15" max="15" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="10" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -604,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -651,12 +654,12 @@
         <v>29</v>
       </c>
       <c r="P2" s="1">
-        <v>65717</v>
+        <v>65728</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -706,13 +709,13 @@
         <v>2</v>
       </c>
       <c r="Q3" s="4">
-        <v>65715</v>
+        <v>65729</v>
       </c>
       <c r="R3" s="4">
-        <v>65716</v>
+        <v>65730</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="15.5">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -720,8 +723,8 @@
       <c r="G4" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Refactorización de la question VerificarContraordenConRango, se agrega el parametro tipo cheque para al taget LBL_CUENTA_ASOCIADA para la validación
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/cheque/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5F52FC-6908-44B9-A2EF-B0FA1FC3F655}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -128,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,27 +532,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" customWidth="1"/>
-    <col min="15" max="15" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="7" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="10" width="23.453125" customWidth="1"/>
+    <col min="11" max="11" width="20.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="15" max="15" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -607,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -654,12 +655,12 @@
         <v>29</v>
       </c>
       <c r="P2" s="1">
-        <v>65728</v>
+        <v>65734</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -709,13 +710,13 @@
         <v>2</v>
       </c>
       <c r="Q3" s="4">
-        <v>65729</v>
+        <v>65735</v>
       </c>
       <c r="R3" s="4">
-        <v>65730</v>
+        <v>65736</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="15.5">
       <c r="B4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -724,7 +725,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Se refactoriza el mapeo de la clase chequeLocator
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/cheque/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA095A-BEB8-435E-A8AF-56346A57D3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -128,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,27 +532,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" customWidth="1"/>
-    <col min="15" max="15" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="7" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="10" width="23.453125" customWidth="1"/>
+    <col min="11" max="11" width="20.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" customWidth="1"/>
+    <col min="15" max="15" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -607,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -654,12 +655,12 @@
         <v>29</v>
       </c>
       <c r="P2" s="1">
-        <v>65740</v>
+        <v>65765</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -706,13 +707,13 @@
         <v>30</v>
       </c>
       <c r="Q3" s="4">
-        <v>65735</v>
+        <v>65762</v>
       </c>
       <c r="R3" s="4">
-        <v>65736</v>
+        <v>65763</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="15.5">
       <c r="B4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -721,7 +722,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Cambios para estabilización de transacciones en IOS
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/cheque/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA095A-BEB8-435E-A8AF-56346A57D3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -129,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,27 +531,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="10" width="23.453125" customWidth="1"/>
-    <col min="11" max="11" width="20.6328125" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
-    <col min="15" max="15" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="10" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -608,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -655,12 +654,12 @@
         <v>29</v>
       </c>
       <c r="P2" s="1">
-        <v>65765</v>
+        <v>65785</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -707,13 +706,13 @@
         <v>30</v>
       </c>
       <c r="Q3" s="4">
-        <v>65762</v>
+        <v>65772</v>
       </c>
       <c r="R3" s="4">
-        <v>65763</v>
+        <v>65773</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="15.5">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -722,7 +721,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
solucion transacciones despues de ajecucion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/cheque/contraordenarcheque.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\cheque\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -648,7 +648,7 @@
         <v>31</v>
       </c>
       <c r="P2" s="3">
-        <v>65805</v>
+        <v>65700</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>

</xml_diff>